<commit_message>
ALU improvment an test for CLAC READ ADD SUB R_SHIFT L_SHIFT and JPNZ opcodes
</commit_message>
<xml_diff>
--- a/Design Documants/Signaling Chart.xlsx
+++ b/Design Documants/Signaling Chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="67">
   <si>
     <t>STATE</t>
   </si>
@@ -83,30 +83,15 @@
     <t>MEM4</t>
   </si>
   <si>
-    <t>WRITE</t>
-  </si>
-  <si>
-    <t>ADD</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
-    <t>SUB</t>
-  </si>
-  <si>
     <t>010</t>
   </si>
   <si>
-    <t>SHIFT</t>
-  </si>
-  <si>
     <t>100</t>
   </si>
   <si>
-    <t>INC</t>
-  </si>
-  <si>
     <t>011</t>
   </si>
   <si>
@@ -216,6 +201,30 @@
   </si>
   <si>
     <t>Control Signals</t>
+  </si>
+  <si>
+    <t>WRITE1</t>
+  </si>
+  <si>
+    <t>CLAC1</t>
+  </si>
+  <si>
+    <t>ADD1</t>
+  </si>
+  <si>
+    <t>SUB1</t>
+  </si>
+  <si>
+    <t>R_SHIFT1</t>
+  </si>
+  <si>
+    <t>L_SHIFT1</t>
+  </si>
+  <si>
+    <t>INC1</t>
+  </si>
+  <si>
+    <t>00100000000101</t>
   </si>
 </sst>
 </file>
@@ -624,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B7:S27"/>
+  <dimension ref="B7:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,19 +680,19 @@
         <v>4</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>5</v>
@@ -698,7 +707,7 @@
         <v>8</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
@@ -747,7 +756,7 @@
       </c>
       <c r="R8" s="3"/>
       <c r="S8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
@@ -796,7 +805,7 @@
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
@@ -845,7 +854,7 @@
       </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
@@ -894,7 +903,7 @@
       </c>
       <c r="R11" s="3"/>
       <c r="S11" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
@@ -943,7 +952,7 @@
       </c>
       <c r="R12" s="3"/>
       <c r="S12" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
@@ -992,7 +1001,7 @@
       </c>
       <c r="R13" s="3"/>
       <c r="S13" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
@@ -1041,7 +1050,7 @@
       </c>
       <c r="R14" s="3"/>
       <c r="S14" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
@@ -1049,7 +1058,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
@@ -1090,7 +1099,7 @@
       </c>
       <c r="R15" s="3"/>
       <c r="S15" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
@@ -1098,7 +1107,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
@@ -1139,7 +1148,7 @@
       </c>
       <c r="R16" s="3"/>
       <c r="S16" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
@@ -1147,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
@@ -1188,7 +1197,7 @@
       </c>
       <c r="R17" s="3"/>
       <c r="S17" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -1196,7 +1205,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
@@ -1237,7 +1246,7 @@
       </c>
       <c r="R18" s="3"/>
       <c r="S18" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -1245,7 +1254,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
@@ -1282,11 +1291,11 @@
         <v>10</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
@@ -1294,7 +1303,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
@@ -1331,11 +1340,11 @@
         <v>10</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R20" s="3"/>
       <c r="S20" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
@@ -1343,7 +1352,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
@@ -1380,11 +1389,11 @@
         <v>10</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="R21" s="3"/>
       <c r="S21" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -1392,7 +1401,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
@@ -1429,11 +1438,11 @@
         <v>10</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="R22" s="3"/>
       <c r="S22" s="3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -1441,17 +1450,17 @@
         <v>16</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="3">
-        <v>1</v>
+      <c r="G23" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>10</v>
@@ -1478,11 +1487,11 @@
         <v>10</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="R23" s="3"/>
       <c r="S23" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -1490,14 +1499,14 @@
         <v>17</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>10</v>
+      <c r="F24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>10</v>
@@ -1531,7 +1540,7 @@
       </c>
       <c r="R24" s="3"/>
       <c r="S24" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -1539,7 +1548,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3">
@@ -1580,48 +1589,97 @@
       </c>
       <c r="R25" s="3"/>
       <c r="S25" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N27" s="5">
+      <c r="K28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="5">
         <v>5</v>
       </c>
-      <c r="O27" s="5">
+      <c r="O28" s="5">
         <v>4</v>
       </c>
-      <c r="P27" s="5">
+      <c r="P28" s="5">
         <v>3</v>
       </c>
-      <c r="Q27" s="5" t="s">
-        <v>32</v>
+      <c r="Q28" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>